<commit_message>
Add names em Periodo
</commit_message>
<xml_diff>
--- a/data/DicionarioDados.xlsx
+++ b/data/DicionarioDados.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nuvem\Google Drive\Grad_Esp_Mest_Dout\4-DOUTORADO\PhD Rodrigo\7. Experimentos\1. Bases de Dados\4. Extração das Variáveis - SRL\Outros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\atividade2Shiny\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Variaveis Comportamentais" sheetId="1" r:id="rId1"/>
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>